<commit_message>
Update RQ1 outputs and add geometric mean analysis
</commit_message>
<xml_diff>
--- a/data/raw/PSY_adolescents.xlsx
+++ b/data/raw/PSY_adolescents.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\giaco\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\giaco\Desktop\Git_META\META\data\raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23321369-A16A-459C-8619-1DCD2AEADE53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9912C7B4-E0C5-419D-9767-3F9AD2645FB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="141">
   <si>
     <t>ASD</t>
   </si>
@@ -303,6 +303,162 @@
   </si>
   <si>
     <t>0.10</t>
+  </si>
+  <si>
+    <t>0.002</t>
+  </si>
+  <si>
+    <t>-0.184</t>
+  </si>
+  <si>
+    <t>-0.092</t>
+  </si>
+  <si>
+    <t>-0.305</t>
+  </si>
+  <si>
+    <t>-0.124</t>
+  </si>
+  <si>
+    <t>-0.256</t>
+  </si>
+  <si>
+    <t>0.099</t>
+  </si>
+  <si>
+    <t>-0.068</t>
+  </si>
+  <si>
+    <t>-0.075</t>
+  </si>
+  <si>
+    <t>-0.083</t>
+  </si>
+  <si>
+    <t>-0.039</t>
+  </si>
+  <si>
+    <t>-0.11</t>
+  </si>
+  <si>
+    <t>-0.063</t>
+  </si>
+  <si>
+    <t>-0.017</t>
+  </si>
+  <si>
+    <t>-0.143</t>
+  </si>
+  <si>
+    <t>-0.132</t>
+  </si>
+  <si>
+    <t>-0.099</t>
+  </si>
+  <si>
+    <t>0.077</t>
+  </si>
+  <si>
+    <t>-0.241</t>
+  </si>
+  <si>
+    <t>0.012</t>
+  </si>
+  <si>
+    <t>-0.152</t>
+  </si>
+  <si>
+    <t>-0.044</t>
+  </si>
+  <si>
+    <t>0.0289999999999999</t>
+  </si>
+  <si>
+    <t>-0.098</t>
+  </si>
+  <si>
+    <t>-0.004</t>
+  </si>
+  <si>
+    <t>0.065</t>
+  </si>
+  <si>
+    <t>-0.133</t>
+  </si>
+  <si>
+    <t>-0.157</t>
+  </si>
+  <si>
+    <t>-0.019</t>
+  </si>
+  <si>
+    <t>-0.067</t>
+  </si>
+  <si>
+    <t>-0.225</t>
+  </si>
+  <si>
+    <t>-0.036</t>
+  </si>
+  <si>
+    <t>0.006</t>
+  </si>
+  <si>
+    <t>-0.078</t>
+  </si>
+  <si>
+    <t>-0.071</t>
+  </si>
+  <si>
+    <t>-0.047</t>
+  </si>
+  <si>
+    <t>-0.0559999999999999</t>
+  </si>
+  <si>
+    <t>-0.096</t>
+  </si>
+  <si>
+    <t>-0.1009999999999999</t>
+  </si>
+  <si>
+    <t>-0.079</t>
+  </si>
+  <si>
+    <t>-0.072</t>
+  </si>
+  <si>
+    <t>-0.076</t>
+  </si>
+  <si>
+    <t>-0.061</t>
+  </si>
+  <si>
+    <t>-0.2689999999999999</t>
+  </si>
+  <si>
+    <t>-0.038</t>
+  </si>
+  <si>
+    <t>-0.073</t>
+  </si>
+  <si>
+    <t>0.042</t>
+  </si>
+  <si>
+    <t>-0.089</t>
+  </si>
+  <si>
+    <t>0.142</t>
+  </si>
+  <si>
+    <t>0.046</t>
+  </si>
+  <si>
+    <t>-0.013</t>
+  </si>
+  <si>
+    <t>0.239</t>
   </si>
 </sst>
 </file>
@@ -644,8 +800,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E83"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="H75" sqref="H75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -681,7 +837,7 @@
         <v>39</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>59</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -698,7 +854,7 @@
         <v>39</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>19</v>
+        <v>89</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -715,7 +871,7 @@
         <v>71</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -732,7 +888,7 @@
         <v>71</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>19</v>
+        <v>90</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -749,7 +905,7 @@
         <v>69</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>58</v>
+        <v>78</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -766,7 +922,7 @@
         <v>69</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>61</v>
+        <v>91</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -783,7 +939,7 @@
         <v>72</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>15</v>
+        <v>92</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -800,7 +956,7 @@
         <v>72</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>15</v>
+        <v>53</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -817,7 +973,7 @@
         <v>73</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>10</v>
+        <v>93</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -834,7 +990,7 @@
         <v>73</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>23</v>
+        <v>94</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -851,7 +1007,7 @@
         <v>74</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>4</v>
+        <v>95</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -868,7 +1024,7 @@
         <v>74</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>15</v>
+        <v>96</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -885,7 +1041,7 @@
         <v>75</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>10</v>
+        <v>97</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -902,7 +1058,7 @@
         <v>75</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>60</v>
+        <v>98</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -919,7 +1075,7 @@
         <v>37</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>62</v>
+        <v>99</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -936,7 +1092,7 @@
         <v>37</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>58</v>
+        <v>100</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -953,7 +1109,7 @@
         <v>69</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>60</v>
+        <v>101</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -970,7 +1126,7 @@
         <v>69</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>4</v>
+        <v>102</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -986,8 +1142,8 @@
       <c r="D20" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="E20" s="3">
-        <v>0</v>
+      <c r="E20" s="3" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -1004,7 +1160,7 @@
         <v>67</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>21</v>
+        <v>103</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -1021,7 +1177,7 @@
         <v>76</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>15</v>
+        <v>53</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -1037,8 +1193,8 @@
       <c r="D23" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="E23" s="3">
-        <v>0</v>
+      <c r="E23" s="3" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -1055,7 +1211,7 @@
         <v>42</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>63</v>
+        <v>105</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -1072,7 +1228,7 @@
         <v>42</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -1089,7 +1245,7 @@
         <v>77</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>64</v>
+        <v>106</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
@@ -1106,7 +1262,7 @@
         <v>77</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>7</v>
+        <v>36</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -1123,7 +1279,7 @@
         <v>78</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>6</v>
+        <v>59</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -1140,7 +1296,7 @@
         <v>78</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>60</v>
+        <v>107</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
@@ -1157,7 +1313,7 @@
         <v>78</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>4</v>
+        <v>108</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
@@ -1174,7 +1330,7 @@
         <v>78</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>60</v>
+        <v>109</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
@@ -1191,7 +1347,7 @@
         <v>79</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>19</v>
+        <v>110</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
@@ -1208,7 +1364,7 @@
         <v>79</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>65</v>
+        <v>111</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
@@ -1225,7 +1381,7 @@
         <v>80</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>64</v>
+        <v>112</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
@@ -1242,7 +1398,7 @@
         <v>80</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>58</v>
+        <v>113</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
@@ -1259,7 +1415,7 @@
         <v>69</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>59</v>
+        <v>100</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
@@ -1276,7 +1432,7 @@
         <v>69</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>19</v>
+        <v>114</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
@@ -1293,7 +1449,7 @@
         <v>67</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>60</v>
+        <v>115</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
@@ -1310,7 +1466,7 @@
         <v>67</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>19</v>
+        <v>116</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
@@ -1327,7 +1483,7 @@
         <v>77</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>58</v>
+        <v>117</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
@@ -1344,7 +1500,7 @@
         <v>77</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>61</v>
+        <v>118</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
@@ -1361,7 +1517,7 @@
         <v>75</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>15</v>
+        <v>119</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
@@ -1378,7 +1534,7 @@
         <v>75</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>15</v>
+        <v>98</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
@@ -1395,7 +1551,7 @@
         <v>78</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>10</v>
+        <v>120</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
@@ -1412,7 +1568,7 @@
         <v>78</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
@@ -1429,7 +1585,7 @@
         <v>81</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
@@ -1446,7 +1602,7 @@
         <v>81</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>15</v>
+        <v>121</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
@@ -1463,7 +1619,7 @@
         <v>77</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>10</v>
+        <v>38</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
@@ -1480,7 +1636,7 @@
         <v>77</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>60</v>
+        <v>122</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
@@ -1497,7 +1653,7 @@
         <v>82</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>62</v>
+        <v>96</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
@@ -1514,7 +1670,7 @@
         <v>82</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>58</v>
+        <v>123</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
@@ -1531,7 +1687,7 @@
         <v>68</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>60</v>
+        <v>99</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
@@ -1548,7 +1704,7 @@
         <v>68</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>4</v>
+        <v>124</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
@@ -1564,8 +1720,8 @@
       <c r="D54" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="E54" s="3">
-        <v>0</v>
+      <c r="E54" s="3" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
@@ -1582,7 +1738,7 @@
         <v>83</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
@@ -1599,7 +1755,7 @@
         <v>81</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>15</v>
+        <v>126</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
@@ -1615,8 +1771,8 @@
       <c r="D57" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="E57" s="3">
-        <v>0</v>
+      <c r="E57" s="3" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
@@ -1633,7 +1789,7 @@
         <v>84</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>63</v>
+        <v>128</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
@@ -1650,7 +1806,7 @@
         <v>84</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>23</v>
+        <v>109</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
@@ -1667,7 +1823,7 @@
         <v>74</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>64</v>
+        <v>129</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
@@ -1684,7 +1840,7 @@
         <v>74</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>7</v>
+        <v>130</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
@@ -1701,7 +1857,7 @@
         <v>79</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>6</v>
+        <v>131</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
@@ -1718,7 +1874,7 @@
         <v>79</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>60</v>
+        <v>132</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
@@ -1735,7 +1891,7 @@
         <v>37</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>4</v>
+        <v>133</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
@@ -1752,7 +1908,7 @@
         <v>37</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>60</v>
+        <v>134</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
@@ -1769,7 +1925,7 @@
         <v>70</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>19</v>
+        <v>135</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
@@ -1786,7 +1942,7 @@
         <v>70</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>65</v>
+        <v>47</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
@@ -1803,7 +1959,7 @@
         <v>69</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>64</v>
+        <v>35</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
@@ -1820,7 +1976,7 @@
         <v>69</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>58</v>
+        <v>136</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
@@ -1837,7 +1993,7 @@
         <v>-0.13</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
@@ -1854,7 +2010,7 @@
         <v>-0.08</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>65</v>
+        <v>137</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
@@ -1871,7 +2027,7 @@
         <v>-0.04</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>18</v>
+        <v>138</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
@@ -1888,7 +2044,7 @@
         <v>-0.1</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>12</v>
+        <v>64</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
@@ -1905,7 +2061,7 @@
         <v>0.01</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>6</v>
+        <v>93</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
@@ -1922,7 +2078,7 @@
         <v>-0.05</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>65</v>
+        <v>139</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
@@ -1939,7 +2095,7 @@
         <v>-0.15</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>13</v>
+        <v>140</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
@@ -1956,7 +2112,7 @@
         <v>-0.08</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
@@ -1973,7 +2129,7 @@
         <v>-0.15</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>65</v>
+        <v>137</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
@@ -1990,7 +2146,7 @@
         <v>-0.05</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>18</v>
+        <v>138</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
@@ -2007,7 +2163,7 @@
         <v>-0.13</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>12</v>
+        <v>64</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
@@ -2024,7 +2180,7 @@
         <v>-0.01</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>6</v>
+        <v>93</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
@@ -2041,7 +2197,7 @@
         <v>-0.02</v>
       </c>
       <c r="E82" s="1" t="s">
-        <v>65</v>
+        <v>139</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
@@ -2058,7 +2214,7 @@
         <v>-0.11</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>13</v>
+        <v>140</v>
       </c>
     </row>
   </sheetData>

</xml_diff>